<commit_message>
built out preprocess residents
</commit_message>
<xml_diff>
--- a/data/residents/2020-PD-Survey_sub.xlsx
+++ b/data/residents/2020-PD-Survey_sub.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">Specialty</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent Citing Factor</t>
+    <t xml:space="preserve">Factor</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent citing factor</t>
+    <t xml:space="preserve">Percent Citing Factor</t>
   </si>
   <si>
     <t xml:space="preserve">Average Rating</t>
@@ -175,9 +175,6 @@
     <t xml:space="preserve">Internal Medicine/Pediatrics</t>
   </si>
   <si>
-    <t xml:space="preserve">USMLE Step 1 score 100%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Medical Student Performance Evaluation (MSPE/Dean's Letter) </t>
   </si>
   <si>
@@ -214,6 +211,9 @@
     <t xml:space="preserve">Physical Medicine and Rehabilitation</t>
   </si>
   <si>
+    <t xml:space="preserve">Plastic Surgery</t>
+  </si>
+  <si>
     <t xml:space="preserve">Psychiatry</t>
   </si>
   <si>
@@ -243,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -264,12 +264,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -320,7 +314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,7 +322,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -351,11 +345,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A200" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A230" activeCellId="0" sqref="A230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.39"/>
@@ -3566,7 +3560,7 @@
         <v>50</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C230" s="2" t="n">
         <v>1</v>
@@ -3622,7 +3616,7 @@
         <v>50</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C234" s="1" t="n">
         <v>1</v>
@@ -4092,7 +4086,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B268" s="0" t="s">
         <v>44</v>
@@ -4106,10 +4100,10 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B269" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B269" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="C269" s="1" t="n">
         <v>1</v>
@@ -4120,7 +4114,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B270" s="0" t="s">
         <v>7</v>
@@ -4134,7 +4128,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B271" s="0" t="s">
         <v>8</v>
@@ -4148,7 +4142,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B272" s="0" t="s">
         <v>9</v>
@@ -4162,7 +4156,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B273" s="0" t="s">
         <v>10</v>
@@ -4176,7 +4170,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B274" s="0" t="s">
         <v>11</v>
@@ -4190,7 +4184,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B275" s="0" t="s">
         <v>12</v>
@@ -4204,7 +4198,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B276" s="0" t="s">
         <v>13</v>
@@ -4218,7 +4212,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B277" s="0" t="s">
         <v>14</v>
@@ -4232,10 +4226,10 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B278" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C278" s="1" t="n">
         <v>1</v>
@@ -4246,7 +4240,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B279" s="0" t="s">
         <v>16</v>
@@ -4260,7 +4254,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B280" s="0" t="s">
         <v>17</v>
@@ -4274,7 +4268,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B281" s="0" t="s">
         <v>18</v>
@@ -4288,7 +4282,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B282" s="0" t="s">
         <v>19</v>
@@ -4302,7 +4296,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B283" s="0" t="s">
         <v>20</v>
@@ -4316,7 +4310,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B284" s="0" t="s">
         <v>21</v>
@@ -4330,7 +4324,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B285" s="0" t="s">
         <v>22</v>
@@ -4344,7 +4338,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B286" s="0" t="s">
         <v>23</v>
@@ -4358,7 +4352,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B287" s="0" t="s">
         <v>24</v>
@@ -4372,7 +4366,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B288" s="0" t="s">
         <v>25</v>
@@ -4386,7 +4380,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B289" s="0" t="s">
         <v>26</v>
@@ -4400,7 +4394,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B290" s="0" t="s">
         <v>27</v>
@@ -4414,7 +4408,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B291" s="0" t="s">
         <v>28</v>
@@ -4428,7 +4422,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B292" s="0" t="s">
         <v>29</v>
@@ -4442,7 +4436,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B293" s="0" t="s">
         <v>30</v>
@@ -4456,7 +4450,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B294" s="0" t="s">
         <v>31</v>
@@ -4470,7 +4464,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B295" s="0" t="s">
         <v>32</v>
@@ -4484,7 +4478,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B296" s="0" t="s">
         <v>33</v>
@@ -4498,7 +4492,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B297" s="0" t="s">
         <v>34</v>
@@ -4512,7 +4506,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B298" s="0" t="s">
         <v>35</v>
@@ -4526,7 +4520,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B299" s="0" t="s">
         <v>36</v>
@@ -4540,7 +4534,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B300" s="0" t="s">
         <v>37</v>
@@ -4554,7 +4548,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B301" s="0" t="s">
         <v>38</v>
@@ -4568,7 +4562,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B302" s="0" t="s">
         <v>39</v>
@@ -4582,7 +4576,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B303" s="0" t="s">
         <v>40</v>
@@ -4596,7 +4590,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B304" s="0" t="s">
         <v>41</v>
@@ -4610,7 +4604,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B305" s="0" t="s">
         <v>42</v>
@@ -4624,7 +4618,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B306" s="0" t="s">
         <v>44</v>
@@ -4638,7 +4632,7 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B307" s="0" t="s">
         <v>6</v>
@@ -4652,7 +4646,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B308" s="0" t="s">
         <v>7</v>
@@ -4666,7 +4660,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B309" s="0" t="s">
         <v>8</v>
@@ -4680,7 +4674,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B310" s="0" t="s">
         <v>9</v>
@@ -4694,7 +4688,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B311" s="0" t="s">
         <v>10</v>
@@ -4708,7 +4702,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B312" s="0" t="s">
         <v>11</v>
@@ -4722,7 +4716,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B313" s="0" t="s">
         <v>12</v>
@@ -4736,7 +4730,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B314" s="0" t="s">
         <v>13</v>
@@ -4750,7 +4744,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B315" s="0" t="s">
         <v>14</v>
@@ -4764,7 +4758,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B316" s="0" t="s">
         <v>15</v>
@@ -4778,7 +4772,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B317" s="0" t="s">
         <v>16</v>
@@ -4792,7 +4786,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B318" s="0" t="s">
         <v>17</v>
@@ -4806,7 +4800,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B319" s="0" t="s">
         <v>18</v>
@@ -4820,7 +4814,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B320" s="0" t="s">
         <v>19</v>
@@ -4834,7 +4828,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B321" s="0" t="s">
         <v>20</v>
@@ -4848,7 +4842,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B322" s="0" t="s">
         <v>21</v>
@@ -4862,7 +4856,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B323" s="0" t="s">
         <v>22</v>
@@ -4876,7 +4870,7 @@
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B324" s="0" t="s">
         <v>23</v>
@@ -4890,7 +4884,7 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B325" s="0" t="s">
         <v>24</v>
@@ -4901,7 +4895,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B326" s="0" t="s">
         <v>25</v>
@@ -4915,7 +4909,7 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B327" s="0" t="s">
         <v>26</v>
@@ -4929,7 +4923,7 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B328" s="0" t="s">
         <v>27</v>
@@ -4943,7 +4937,7 @@
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B329" s="0" t="s">
         <v>28</v>
@@ -4957,7 +4951,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B330" s="0" t="s">
         <v>29</v>
@@ -4971,7 +4965,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B331" s="0" t="s">
         <v>30</v>
@@ -4985,7 +4979,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B332" s="0" t="s">
         <v>31</v>
@@ -4999,7 +4993,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B333" s="0" t="s">
         <v>32</v>
@@ -5013,7 +5007,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B334" s="0" t="s">
         <v>33</v>
@@ -5027,7 +5021,7 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B335" s="0" t="s">
         <v>34</v>
@@ -5041,7 +5035,7 @@
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B336" s="0" t="s">
         <v>35</v>
@@ -5055,7 +5049,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B337" s="0" t="s">
         <v>36</v>
@@ -5069,7 +5063,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B338" s="0" t="s">
         <v>37</v>
@@ -5083,7 +5077,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B339" s="0" t="s">
         <v>38</v>
@@ -5097,7 +5091,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B340" s="0" t="s">
         <v>39</v>
@@ -5111,7 +5105,7 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B341" s="0" t="s">
         <v>40</v>
@@ -5125,7 +5119,7 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B342" s="0" t="s">
         <v>41</v>
@@ -5139,7 +5133,7 @@
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B343" s="0" t="s">
         <v>42</v>
@@ -5150,7 +5144,7 @@
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B344" s="0" t="s">
         <v>44</v>
@@ -5164,7 +5158,7 @@
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B345" s="0" t="s">
         <v>6</v>
@@ -5178,7 +5172,7 @@
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B346" s="0" t="s">
         <v>7</v>
@@ -5192,7 +5186,7 @@
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B347" s="0" t="s">
         <v>8</v>
@@ -5206,7 +5200,7 @@
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B348" s="0" t="s">
         <v>9</v>
@@ -5220,7 +5214,7 @@
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B349" s="0" t="s">
         <v>10</v>
@@ -5234,7 +5228,7 @@
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B350" s="0" t="s">
         <v>11</v>
@@ -5248,7 +5242,7 @@
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B351" s="0" t="s">
         <v>12</v>
@@ -5262,7 +5256,7 @@
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B352" s="0" t="s">
         <v>13</v>
@@ -5276,7 +5270,7 @@
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B353" s="0" t="s">
         <v>14</v>
@@ -5290,7 +5284,7 @@
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B354" s="0" t="s">
         <v>15</v>
@@ -5304,7 +5298,7 @@
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B355" s="0" t="s">
         <v>16</v>
@@ -5318,7 +5312,7 @@
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B356" s="0" t="s">
         <v>17</v>
@@ -5332,7 +5326,7 @@
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B357" s="0" t="s">
         <v>18</v>
@@ -5346,7 +5340,7 @@
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B358" s="0" t="s">
         <v>19</v>
@@ -5360,7 +5354,7 @@
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B359" s="0" t="s">
         <v>20</v>
@@ -5374,7 +5368,7 @@
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B360" s="0" t="s">
         <v>21</v>
@@ -5388,7 +5382,7 @@
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B361" s="0" t="s">
         <v>22</v>
@@ -5402,7 +5396,7 @@
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B362" s="0" t="s">
         <v>23</v>
@@ -5416,7 +5410,7 @@
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B363" s="0" t="s">
         <v>24</v>
@@ -5430,7 +5424,7 @@
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B364" s="0" t="s">
         <v>25</v>
@@ -5444,7 +5438,7 @@
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B365" s="0" t="s">
         <v>26</v>
@@ -5458,7 +5452,7 @@
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B366" s="0" t="s">
         <v>27</v>
@@ -5472,7 +5466,7 @@
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B367" s="0" t="s">
         <v>28</v>
@@ -5486,7 +5480,7 @@
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B368" s="0" t="s">
         <v>29</v>
@@ -5500,7 +5494,7 @@
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B369" s="0" t="s">
         <v>30</v>
@@ -5514,7 +5508,7 @@
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B370" s="0" t="s">
         <v>31</v>
@@ -5528,7 +5522,7 @@
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B371" s="0" t="s">
         <v>32</v>
@@ -5542,7 +5536,7 @@
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B372" s="0" t="s">
         <v>33</v>
@@ -5556,7 +5550,7 @@
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B373" s="0" t="s">
         <v>34</v>
@@ -5570,7 +5564,7 @@
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B374" s="0" t="s">
         <v>35</v>
@@ -5584,7 +5578,7 @@
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B375" s="0" t="s">
         <v>36</v>
@@ -5598,7 +5592,7 @@
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B376" s="0" t="s">
         <v>37</v>
@@ -5612,7 +5606,7 @@
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B377" s="0" t="s">
         <v>38</v>
@@ -5626,7 +5620,7 @@
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B378" s="0" t="s">
         <v>39</v>
@@ -5640,7 +5634,7 @@
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B379" s="0" t="s">
         <v>40</v>
@@ -5654,7 +5648,7 @@
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B380" s="0" t="s">
         <v>41</v>
@@ -5668,7 +5662,7 @@
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B381" s="0" t="s">
         <v>42</v>
@@ -5682,7 +5676,7 @@
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B382" s="0" t="s">
         <v>44</v>
@@ -5696,7 +5690,7 @@
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B383" s="0" t="s">
         <v>6</v>
@@ -5710,7 +5704,7 @@
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B384" s="0" t="s">
         <v>7</v>
@@ -5724,7 +5718,7 @@
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B385" s="0" t="s">
         <v>8</v>
@@ -5738,7 +5732,7 @@
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B386" s="0" t="s">
         <v>9</v>
@@ -5752,7 +5746,7 @@
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B387" s="0" t="s">
         <v>10</v>
@@ -5766,7 +5760,7 @@
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B388" s="0" t="s">
         <v>11</v>
@@ -5780,7 +5774,7 @@
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B389" s="0" t="s">
         <v>12</v>
@@ -5794,7 +5788,7 @@
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B390" s="0" t="s">
         <v>13</v>
@@ -5808,7 +5802,7 @@
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B391" s="0" t="s">
         <v>14</v>
@@ -5822,7 +5816,7 @@
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B392" s="0" t="s">
         <v>15</v>
@@ -5836,7 +5830,7 @@
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B393" s="0" t="s">
         <v>16</v>
@@ -5850,7 +5844,7 @@
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B394" s="0" t="s">
         <v>17</v>
@@ -5864,7 +5858,7 @@
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B395" s="0" t="s">
         <v>18</v>
@@ -5878,7 +5872,7 @@
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B396" s="0" t="s">
         <v>19</v>
@@ -5892,7 +5886,7 @@
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B397" s="0" t="s">
         <v>20</v>
@@ -5906,7 +5900,7 @@
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B398" s="0" t="s">
         <v>21</v>
@@ -5920,7 +5914,7 @@
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B399" s="0" t="s">
         <v>22</v>
@@ -5934,7 +5928,7 @@
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B400" s="0" t="s">
         <v>23</v>
@@ -5948,7 +5942,7 @@
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B401" s="0" t="s">
         <v>24</v>
@@ -5962,7 +5956,7 @@
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B402" s="0" t="s">
         <v>25</v>
@@ -5976,7 +5970,7 @@
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B403" s="0" t="s">
         <v>26</v>
@@ -5990,7 +5984,7 @@
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B404" s="0" t="s">
         <v>27</v>
@@ -6004,7 +5998,7 @@
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B405" s="0" t="s">
         <v>28</v>
@@ -6018,7 +6012,7 @@
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B406" s="0" t="s">
         <v>29</v>
@@ -6032,7 +6026,7 @@
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B407" s="0" t="s">
         <v>30</v>
@@ -6046,7 +6040,7 @@
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B408" s="0" t="s">
         <v>31</v>
@@ -6060,7 +6054,7 @@
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B409" s="0" t="s">
         <v>32</v>
@@ -6074,7 +6068,7 @@
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B410" s="0" t="s">
         <v>33</v>
@@ -6088,7 +6082,7 @@
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B411" s="0" t="s">
         <v>34</v>
@@ -6102,7 +6096,7 @@
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B412" s="0" t="s">
         <v>35</v>
@@ -6116,7 +6110,7 @@
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B413" s="0" t="s">
         <v>36</v>
@@ -6130,7 +6124,7 @@
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B414" s="0" t="s">
         <v>37</v>
@@ -6144,7 +6138,7 @@
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B415" s="0" t="s">
         <v>38</v>
@@ -6158,7 +6152,7 @@
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B416" s="0" t="s">
         <v>39</v>
@@ -6172,7 +6166,7 @@
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B417" s="0" t="s">
         <v>40</v>
@@ -6186,7 +6180,7 @@
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B418" s="0" t="s">
         <v>41</v>
@@ -6200,7 +6194,7 @@
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B419" s="0" t="s">
         <v>42</v>
@@ -6214,7 +6208,7 @@
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B420" s="0" t="s">
         <v>44</v>
@@ -6228,7 +6222,7 @@
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B421" s="0" t="s">
         <v>6</v>
@@ -6242,7 +6236,7 @@
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B422" s="0" t="s">
         <v>7</v>
@@ -6256,7 +6250,7 @@
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B423" s="0" t="s">
         <v>8</v>
@@ -6270,7 +6264,7 @@
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B424" s="0" t="s">
         <v>9</v>
@@ -6284,7 +6278,7 @@
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B425" s="0" t="s">
         <v>10</v>
@@ -6298,7 +6292,7 @@
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B426" s="0" t="s">
         <v>11</v>
@@ -6312,7 +6306,7 @@
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B427" s="0" t="s">
         <v>12</v>
@@ -6326,7 +6320,7 @@
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B428" s="0" t="s">
         <v>13</v>
@@ -6340,7 +6334,7 @@
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B429" s="0" t="s">
         <v>14</v>
@@ -6354,7 +6348,7 @@
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B430" s="0" t="s">
         <v>15</v>
@@ -6368,7 +6362,7 @@
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B431" s="0" t="s">
         <v>16</v>
@@ -6382,7 +6376,7 @@
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B432" s="0" t="s">
         <v>17</v>
@@ -6396,7 +6390,7 @@
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B433" s="0" t="s">
         <v>18</v>
@@ -6410,7 +6404,7 @@
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B434" s="0" t="s">
         <v>19</v>
@@ -6424,7 +6418,7 @@
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B435" s="0" t="s">
         <v>20</v>
@@ -6438,7 +6432,7 @@
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B436" s="0" t="s">
         <v>21</v>
@@ -6452,7 +6446,7 @@
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B437" s="0" t="s">
         <v>22</v>
@@ -6466,7 +6460,7 @@
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B438" s="0" t="s">
         <v>23</v>
@@ -6480,7 +6474,7 @@
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B439" s="0" t="s">
         <v>24</v>
@@ -6494,7 +6488,7 @@
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B440" s="0" t="s">
         <v>25</v>
@@ -6508,7 +6502,7 @@
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B441" s="0" t="s">
         <v>26</v>
@@ -6522,7 +6516,7 @@
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B442" s="0" t="s">
         <v>27</v>
@@ -6536,7 +6530,7 @@
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B443" s="0" t="s">
         <v>28</v>
@@ -6550,7 +6544,7 @@
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B444" s="0" t="s">
         <v>29</v>
@@ -6564,7 +6558,7 @@
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B445" s="0" t="s">
         <v>30</v>
@@ -6578,7 +6572,7 @@
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B446" s="0" t="s">
         <v>31</v>
@@ -6592,7 +6586,7 @@
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B447" s="0" t="s">
         <v>32</v>
@@ -6606,7 +6600,7 @@
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B448" s="0" t="s">
         <v>33</v>
@@ -6620,7 +6614,7 @@
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B449" s="0" t="s">
         <v>34</v>
@@ -6634,7 +6628,7 @@
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B450" s="0" t="s">
         <v>35</v>
@@ -6648,7 +6642,7 @@
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B451" s="0" t="s">
         <v>36</v>
@@ -6662,7 +6656,7 @@
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B452" s="0" t="s">
         <v>37</v>
@@ -6676,7 +6670,7 @@
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B453" s="0" t="s">
         <v>38</v>
@@ -6690,7 +6684,7 @@
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B454" s="0" t="s">
         <v>39</v>
@@ -6704,7 +6698,7 @@
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B455" s="0" t="s">
         <v>40</v>
@@ -6718,7 +6712,7 @@
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B456" s="0" t="s">
         <v>41</v>
@@ -6732,7 +6726,7 @@
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B457" s="0" t="s">
         <v>42</v>
@@ -6743,7 +6737,7 @@
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B458" s="0" t="s">
         <v>44</v>
@@ -6757,7 +6751,7 @@
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B459" s="0" t="s">
         <v>6</v>
@@ -6771,7 +6765,7 @@
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B460" s="0" t="s">
         <v>7</v>
@@ -6785,7 +6779,7 @@
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B461" s="0" t="s">
         <v>8</v>
@@ -6799,7 +6793,7 @@
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B462" s="0" t="s">
         <v>9</v>
@@ -6813,7 +6807,7 @@
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B463" s="0" t="s">
         <v>10</v>
@@ -6827,7 +6821,7 @@
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B464" s="0" t="s">
         <v>11</v>
@@ -6841,7 +6835,7 @@
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B465" s="0" t="s">
         <v>12</v>
@@ -6855,7 +6849,7 @@
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B466" s="0" t="s">
         <v>13</v>
@@ -6869,7 +6863,7 @@
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B467" s="0" t="s">
         <v>14</v>
@@ -6883,7 +6877,7 @@
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B468" s="0" t="s">
         <v>15</v>
@@ -6897,7 +6891,7 @@
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B469" s="0" t="s">
         <v>16</v>
@@ -6911,7 +6905,7 @@
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B470" s="0" t="s">
         <v>17</v>
@@ -6925,7 +6919,7 @@
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B471" s="0" t="s">
         <v>18</v>
@@ -6939,7 +6933,7 @@
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B472" s="0" t="s">
         <v>19</v>
@@ -6953,7 +6947,7 @@
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B473" s="0" t="s">
         <v>20</v>
@@ -6967,7 +6961,7 @@
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B474" s="0" t="s">
         <v>21</v>
@@ -6981,7 +6975,7 @@
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B475" s="0" t="s">
         <v>22</v>
@@ -6995,7 +6989,7 @@
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B476" s="0" t="s">
         <v>23</v>
@@ -7009,7 +7003,7 @@
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B477" s="0" t="s">
         <v>24</v>
@@ -7023,7 +7017,7 @@
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B478" s="0" t="s">
         <v>25</v>
@@ -7037,7 +7031,7 @@
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B479" s="0" t="s">
         <v>26</v>
@@ -7051,7 +7045,7 @@
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B480" s="0" t="s">
         <v>27</v>
@@ -7065,7 +7059,7 @@
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B481" s="0" t="s">
         <v>28</v>
@@ -7079,7 +7073,7 @@
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B482" s="0" t="s">
         <v>29</v>
@@ -7093,7 +7087,7 @@
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B483" s="0" t="s">
         <v>30</v>
@@ -7107,7 +7101,7 @@
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B484" s="0" t="s">
         <v>31</v>
@@ -7121,7 +7115,7 @@
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B485" s="0" t="s">
         <v>32</v>
@@ -7135,7 +7129,7 @@
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B486" s="0" t="s">
         <v>33</v>
@@ -7149,7 +7143,7 @@
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B487" s="0" t="s">
         <v>34</v>
@@ -7163,7 +7157,7 @@
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B488" s="0" t="s">
         <v>35</v>
@@ -7177,7 +7171,7 @@
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B489" s="0" t="s">
         <v>36</v>
@@ -7191,7 +7185,7 @@
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B490" s="0" t="s">
         <v>37</v>
@@ -7205,7 +7199,7 @@
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B491" s="0" t="s">
         <v>38</v>
@@ -7216,7 +7210,7 @@
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B492" s="0" t="s">
         <v>39</v>
@@ -7230,7 +7224,7 @@
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B493" s="0" t="s">
         <v>40</v>
@@ -7244,7 +7238,7 @@
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B494" s="0" t="s">
         <v>41</v>
@@ -7258,7 +7252,7 @@
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B495" s="0" t="s">
         <v>42</v>
@@ -7272,7 +7266,7 @@
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B496" s="0" t="s">
         <v>44</v>
@@ -7286,7 +7280,7 @@
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B497" s="0" t="s">
         <v>6</v>
@@ -7300,7 +7294,7 @@
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B498" s="0" t="s">
         <v>7</v>
@@ -7314,7 +7308,7 @@
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B499" s="0" t="s">
         <v>8</v>
@@ -7328,7 +7322,7 @@
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B500" s="0" t="s">
         <v>9</v>
@@ -7342,7 +7336,7 @@
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B501" s="0" t="s">
         <v>10</v>
@@ -7356,7 +7350,7 @@
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B502" s="0" t="s">
         <v>11</v>
@@ -7370,7 +7364,7 @@
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B503" s="0" t="s">
         <v>12</v>
@@ -7384,7 +7378,7 @@
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B504" s="0" t="s">
         <v>13</v>
@@ -7398,7 +7392,7 @@
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B505" s="0" t="s">
         <v>14</v>
@@ -7412,7 +7406,7 @@
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B506" s="0" t="s">
         <v>15</v>
@@ -7426,7 +7420,7 @@
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B507" s="0" t="s">
         <v>16</v>
@@ -7440,7 +7434,7 @@
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B508" s="0" t="s">
         <v>17</v>
@@ -7454,7 +7448,7 @@
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B509" s="0" t="s">
         <v>18</v>
@@ -7468,7 +7462,7 @@
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B510" s="0" t="s">
         <v>19</v>
@@ -7482,7 +7476,7 @@
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B511" s="0" t="s">
         <v>20</v>
@@ -7496,7 +7490,7 @@
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B512" s="0" t="s">
         <v>21</v>
@@ -7510,7 +7504,7 @@
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B513" s="0" t="s">
         <v>22</v>
@@ -7524,7 +7518,7 @@
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B514" s="0" t="s">
         <v>23</v>
@@ -7538,7 +7532,7 @@
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B515" s="0" t="s">
         <v>24</v>
@@ -7552,7 +7546,7 @@
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B516" s="0" t="s">
         <v>25</v>
@@ -7566,7 +7560,7 @@
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B517" s="0" t="s">
         <v>26</v>
@@ -7580,7 +7574,7 @@
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B518" s="0" t="s">
         <v>27</v>
@@ -7594,7 +7588,7 @@
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B519" s="0" t="s">
         <v>28</v>
@@ -7608,7 +7602,7 @@
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B520" s="0" t="s">
         <v>29</v>
@@ -7622,7 +7616,7 @@
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B521" s="0" t="s">
         <v>30</v>
@@ -7636,7 +7630,7 @@
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B522" s="0" t="s">
         <v>31</v>
@@ -7650,7 +7644,7 @@
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B523" s="0" t="s">
         <v>32</v>
@@ -7664,7 +7658,7 @@
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B524" s="0" t="s">
         <v>33</v>
@@ -7678,7 +7672,7 @@
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B525" s="0" t="s">
         <v>34</v>
@@ -7692,7 +7686,7 @@
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B526" s="0" t="s">
         <v>35</v>
@@ -7706,7 +7700,7 @@
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B527" s="0" t="s">
         <v>36</v>
@@ -7720,7 +7714,7 @@
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B528" s="0" t="s">
         <v>37</v>
@@ -7734,7 +7728,7 @@
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B529" s="0" t="s">
         <v>38</v>
@@ -7748,7 +7742,7 @@
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B530" s="0" t="s">
         <v>39</v>
@@ -7762,7 +7756,7 @@
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B531" s="0" t="s">
         <v>40</v>
@@ -7776,7 +7770,7 @@
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B532" s="0" t="s">
         <v>41</v>
@@ -7790,7 +7784,7 @@
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B533" s="0" t="s">
         <v>42</v>
@@ -7804,7 +7798,7 @@
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B534" s="0" t="s">
         <v>44</v>
@@ -7818,7 +7812,7 @@
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B535" s="0" t="s">
         <v>6</v>
@@ -7832,7 +7826,7 @@
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B536" s="0" t="s">
         <v>7</v>
@@ -7846,7 +7840,7 @@
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B537" s="0" t="s">
         <v>8</v>
@@ -7860,7 +7854,7 @@
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B538" s="0" t="s">
         <v>9</v>
@@ -7874,7 +7868,7 @@
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B539" s="0" t="s">
         <v>10</v>
@@ -7888,7 +7882,7 @@
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B540" s="0" t="s">
         <v>11</v>
@@ -7902,7 +7896,7 @@
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B541" s="0" t="s">
         <v>12</v>
@@ -7916,7 +7910,7 @@
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B542" s="0" t="s">
         <v>13</v>
@@ -7930,7 +7924,7 @@
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B543" s="0" t="s">
         <v>14</v>
@@ -7944,7 +7938,7 @@
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B544" s="0" t="s">
         <v>15</v>
@@ -7958,7 +7952,7 @@
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B545" s="0" t="s">
         <v>16</v>
@@ -7972,7 +7966,7 @@
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B546" s="0" t="s">
         <v>17</v>
@@ -7986,7 +7980,7 @@
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B547" s="0" t="s">
         <v>18</v>
@@ -8000,7 +7994,7 @@
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B548" s="0" t="s">
         <v>19</v>
@@ -8014,7 +8008,7 @@
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B549" s="0" t="s">
         <v>20</v>
@@ -8028,7 +8022,7 @@
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B550" s="0" t="s">
         <v>21</v>
@@ -8042,7 +8036,7 @@
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B551" s="0" t="s">
         <v>22</v>
@@ -8056,7 +8050,7 @@
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B552" s="0" t="s">
         <v>23</v>
@@ -8070,7 +8064,7 @@
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B553" s="0" t="s">
         <v>24</v>
@@ -8084,7 +8078,7 @@
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B554" s="0" t="s">
         <v>25</v>
@@ -8098,7 +8092,7 @@
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B555" s="0" t="s">
         <v>26</v>
@@ -8112,7 +8106,7 @@
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B556" s="0" t="s">
         <v>27</v>
@@ -8126,7 +8120,7 @@
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B557" s="0" t="s">
         <v>28</v>
@@ -8140,7 +8134,7 @@
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B558" s="0" t="s">
         <v>29</v>
@@ -8154,7 +8148,7 @@
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B559" s="0" t="s">
         <v>30</v>
@@ -8168,7 +8162,7 @@
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B560" s="0" t="s">
         <v>31</v>
@@ -8182,7 +8176,7 @@
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B561" s="0" t="s">
         <v>32</v>
@@ -8196,7 +8190,7 @@
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B562" s="0" t="s">
         <v>33</v>
@@ -8210,7 +8204,7 @@
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B563" s="0" t="s">
         <v>34</v>
@@ -8224,7 +8218,7 @@
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B564" s="0" t="s">
         <v>35</v>
@@ -8238,7 +8232,7 @@
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B565" s="0" t="s">
         <v>36</v>
@@ -8252,7 +8246,7 @@
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B566" s="0" t="s">
         <v>37</v>
@@ -8266,7 +8260,7 @@
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B567" s="0" t="s">
         <v>38</v>
@@ -8280,7 +8274,7 @@
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B568" s="0" t="s">
         <v>39</v>
@@ -8294,7 +8288,7 @@
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B569" s="0" t="s">
         <v>40</v>
@@ -8308,7 +8302,7 @@
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B570" s="0" t="s">
         <v>41</v>
@@ -8322,7 +8316,7 @@
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B571" s="0" t="s">
         <v>42</v>
@@ -8336,7 +8330,7 @@
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B572" s="0" t="s">
         <v>44</v>
@@ -8350,7 +8344,7 @@
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B573" s="0" t="s">
         <v>6</v>
@@ -8364,7 +8358,7 @@
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B574" s="0" t="s">
         <v>7</v>
@@ -8378,7 +8372,7 @@
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B575" s="0" t="s">
         <v>8</v>
@@ -8392,7 +8386,7 @@
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B576" s="0" t="s">
         <v>9</v>
@@ -8406,7 +8400,7 @@
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B577" s="0" t="s">
         <v>10</v>
@@ -8420,7 +8414,7 @@
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B578" s="0" t="s">
         <v>11</v>
@@ -8434,7 +8428,7 @@
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B579" s="0" t="s">
         <v>12</v>
@@ -8448,7 +8442,7 @@
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B580" s="0" t="s">
         <v>13</v>
@@ -8462,7 +8456,7 @@
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B581" s="0" t="s">
         <v>14</v>
@@ -8476,7 +8470,7 @@
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B582" s="0" t="s">
         <v>15</v>
@@ -8490,7 +8484,7 @@
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B583" s="0" t="s">
         <v>16</v>
@@ -8504,7 +8498,7 @@
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B584" s="0" t="s">
         <v>17</v>
@@ -8518,7 +8512,7 @@
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B585" s="0" t="s">
         <v>18</v>
@@ -8532,7 +8526,7 @@
     </row>
     <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B586" s="0" t="s">
         <v>19</v>
@@ -8546,7 +8540,7 @@
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B587" s="0" t="s">
         <v>20</v>
@@ -8560,7 +8554,7 @@
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B588" s="0" t="s">
         <v>21</v>
@@ -8574,7 +8568,7 @@
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B589" s="0" t="s">
         <v>22</v>
@@ -8588,7 +8582,7 @@
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B590" s="0" t="s">
         <v>23</v>
@@ -8602,7 +8596,7 @@
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B591" s="0" t="s">
         <v>24</v>
@@ -8616,7 +8610,7 @@
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B592" s="0" t="s">
         <v>25</v>
@@ -8630,7 +8624,7 @@
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B593" s="0" t="s">
         <v>26</v>
@@ -8644,7 +8638,7 @@
     </row>
     <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B594" s="0" t="s">
         <v>27</v>
@@ -8658,7 +8652,7 @@
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B595" s="0" t="s">
         <v>28</v>
@@ -8672,7 +8666,7 @@
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B596" s="0" t="s">
         <v>29</v>
@@ -8686,7 +8680,7 @@
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B597" s="0" t="s">
         <v>30</v>
@@ -8700,7 +8694,7 @@
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B598" s="0" t="s">
         <v>31</v>
@@ -8714,7 +8708,7 @@
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B599" s="0" t="s">
         <v>32</v>
@@ -8728,7 +8722,7 @@
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B600" s="0" t="s">
         <v>33</v>
@@ -8742,7 +8736,7 @@
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B601" s="0" t="s">
         <v>34</v>
@@ -8756,7 +8750,7 @@
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B602" s="0" t="s">
         <v>35</v>
@@ -8770,7 +8764,7 @@
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B603" s="0" t="s">
         <v>36</v>
@@ -8784,7 +8778,7 @@
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B604" s="0" t="s">
         <v>37</v>
@@ -8798,7 +8792,7 @@
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B605" s="0" t="s">
         <v>38</v>
@@ -8812,7 +8806,7 @@
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B606" s="0" t="s">
         <v>39</v>
@@ -8826,7 +8820,7 @@
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B607" s="0" t="s">
         <v>40</v>
@@ -8840,7 +8834,7 @@
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B608" s="0" t="s">
         <v>41</v>
@@ -8854,7 +8848,7 @@
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B609" s="0" t="s">
         <v>42</v>

</xml_diff>